<commit_message>
Created loop for running all data input files and converting them to excel files. Then added function that runs the matlab script, updates the excel and then reads it
</commit_message>
<xml_diff>
--- a/Stability/wind_tunnel_test/wind_tunnel_test_matrix.xlsx
+++ b/Stability/wind_tunnel_test/wind_tunnel_test_matrix.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
@@ -491,7 +491,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4">
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5">
@@ -522,10 +522,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>50</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7">
@@ -559,7 +559,7 @@
         <v>50</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8">
@@ -573,10 +573,10 @@
         <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -593,7 +593,7 @@
         <v>200</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10">
@@ -610,7 +610,7 @@
         <v>200</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>12</v>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -638,13 +638,13 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13">
@@ -661,7 +661,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14">
@@ -675,10 +675,10 @@
         <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15">
@@ -692,10 +692,10 @@
         <v>12</v>
       </c>
       <c r="D15" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -712,7 +712,7 @@
         <v>50</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17">
@@ -726,10 +726,10 @@
         <v>12</v>
       </c>
       <c r="D17" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18">
@@ -743,10 +743,10 @@
         <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -763,7 +763,7 @@
         <v>200</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20">
@@ -771,16 +771,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
         <v>12</v>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21">
@@ -788,16 +788,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21" t="n">
         <v>12</v>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -808,13 +808,13 @@
         <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
@@ -828,7 +828,7 @@
         <v>12</v>
       </c>
       <c r="D23" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E23" t="n">
         <v>0.1</v>
@@ -845,7 +845,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E24" t="n">
         <v>0.5</v>
@@ -862,10 +862,10 @@
         <v>12</v>
       </c>
       <c r="D25" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -879,7 +879,7 @@
         <v>12</v>
       </c>
       <c r="D26" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E26" t="n">
         <v>0.1</v>
@@ -896,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="D27" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E27" t="n">
         <v>0.5</v>
@@ -913,10 +913,10 @@
         <v>12</v>
       </c>
       <c r="D28" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -924,13 +924,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C29" t="n">
         <v>12</v>
       </c>
       <c r="D29" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E29" t="n">
         <v>0.1</v>
@@ -941,13 +941,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30" t="n">
         <v>12</v>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E30" t="n">
         <v>0.5</v>
@@ -958,16 +958,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C31" t="n">
         <v>12</v>
       </c>
       <c r="D31" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -978,10 +978,10 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
         <v>0.1</v>
@@ -998,10 +998,10 @@
         <v>12</v>
       </c>
       <c r="D33" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="34">
@@ -1015,10 +1015,10 @@
         <v>12</v>
       </c>
       <c r="D34" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35">
@@ -1032,10 +1032,10 @@
         <v>12</v>
       </c>
       <c r="D35" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1049,10 +1049,10 @@
         <v>12</v>
       </c>
       <c r="D36" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E36" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37">
@@ -1066,10 +1066,10 @@
         <v>12</v>
       </c>
       <c r="D37" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38">
@@ -1077,16 +1077,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38" t="n">
         <v>12</v>
       </c>
       <c r="D38" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E38" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C39" t="n">
         <v>12</v>
       </c>
       <c r="D39" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40">
@@ -1111,16 +1111,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C40" t="n">
         <v>12</v>
       </c>
       <c r="D40" t="n">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41">
@@ -1128,16 +1128,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C41" t="n">
         <v>12</v>
       </c>
       <c r="D41" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>12</v>
       </c>
       <c r="C42" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="43">
@@ -1168,10 +1168,10 @@
         <v>12</v>
       </c>
       <c r="D43" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="44">
@@ -1185,10 +1185,10 @@
         <v>12</v>
       </c>
       <c r="D44" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="45">
@@ -1202,10 +1202,10 @@
         <v>12</v>
       </c>
       <c r="D45" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1219,95 +1219,95 @@
         <v>12</v>
       </c>
       <c r="D46" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E46" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C47" t="n">
         <v>12</v>
       </c>
       <c r="D47" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C48" t="n">
         <v>12</v>
       </c>
       <c r="D48" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C49" t="n">
         <v>12</v>
       </c>
       <c r="D49" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="E49" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C50" t="n">
         <v>12</v>
       </c>
       <c r="D50" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C51" t="n">
         <v>12</v>
       </c>
       <c r="D51" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -1321,10 +1321,10 @@
         <v>12</v>
       </c>
       <c r="D52" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E52" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="53">
@@ -1338,10 +1338,10 @@
         <v>12</v>
       </c>
       <c r="D53" t="n">
-        <v>500</v>
+        <v>2</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="54">
@@ -1355,10 +1355,10 @@
         <v>12</v>
       </c>
       <c r="D54" t="n">
-        <v>500</v>
+        <v>2</v>
       </c>
       <c r="E54" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -1372,10 +1372,10 @@
         <v>12</v>
       </c>
       <c r="D55" t="n">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="E55" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="56">
@@ -1383,16 +1383,16 @@
         <v>3</v>
       </c>
       <c r="B56" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
         <v>12</v>
       </c>
       <c r="D56" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="57">
@@ -1400,16 +1400,16 @@
         <v>3</v>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
         <v>12</v>
       </c>
       <c r="D57" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E57" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1417,7 +1417,7 @@
         <v>3</v>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
         <v>12</v>
@@ -1426,7 +1426,7 @@
         <v>20</v>
       </c>
       <c r="E58" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="59">
@@ -1434,16 +1434,16 @@
         <v>3</v>
       </c>
       <c r="B59" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
         <v>12</v>
       </c>
       <c r="D59" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E59" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="60">
@@ -1451,16 +1451,16 @@
         <v>3</v>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C60" t="n">
         <v>12</v>
       </c>
       <c r="D60" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E60" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1468,7 +1468,7 @@
         <v>3</v>
       </c>
       <c r="B61" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
         <v>12</v>
@@ -1477,7 +1477,7 @@
         <v>100</v>
       </c>
       <c r="E61" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="62">
@@ -1485,16 +1485,16 @@
         <v>3</v>
       </c>
       <c r="B62" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
         <v>12</v>
       </c>
       <c r="D62" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E62" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="63">
@@ -1502,16 +1502,16 @@
         <v>3</v>
       </c>
       <c r="B63" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
         <v>12</v>
       </c>
       <c r="D63" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -1525,10 +1525,10 @@
         <v>12</v>
       </c>
       <c r="D64" t="n">
-        <v>500</v>
+        <v>2</v>
       </c>
       <c r="E64" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="65">
@@ -1536,16 +1536,16 @@
         <v>3</v>
       </c>
       <c r="B65" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C65" t="n">
         <v>12</v>
       </c>
       <c r="D65" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E65" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="66">
@@ -1553,16 +1553,16 @@
         <v>3</v>
       </c>
       <c r="B66" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C66" t="n">
         <v>12</v>
       </c>
       <c r="D66" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1570,16 +1570,16 @@
         <v>3</v>
       </c>
       <c r="B67" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C67" t="n">
         <v>12</v>
       </c>
       <c r="D67" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E67" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="68">
@@ -1587,16 +1587,16 @@
         <v>3</v>
       </c>
       <c r="B68" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C68" t="n">
         <v>12</v>
       </c>
       <c r="D68" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E68" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="69">
@@ -1604,16 +1604,16 @@
         <v>3</v>
       </c>
       <c r="B69" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C69" t="n">
         <v>12</v>
       </c>
       <c r="D69" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E69" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -1621,16 +1621,16 @@
         <v>3</v>
       </c>
       <c r="B70" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C70" t="n">
         <v>12</v>
       </c>
       <c r="D70" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E70" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="71">
@@ -1638,16 +1638,16 @@
         <v>3</v>
       </c>
       <c r="B71" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C71" t="n">
         <v>12</v>
       </c>
       <c r="D71" t="n">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="E71" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72">
@@ -1655,16 +1655,16 @@
         <v>3</v>
       </c>
       <c r="B72" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C72" t="n">
         <v>12</v>
       </c>
       <c r="D72" t="n">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="E72" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -1672,225 +1672,225 @@
         <v>3</v>
       </c>
       <c r="B73" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C73" t="n">
         <v>12</v>
       </c>
       <c r="D73" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E73" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C74" t="n">
         <v>12</v>
       </c>
       <c r="D74" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E74" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C75" t="n">
         <v>12</v>
       </c>
       <c r="D75" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E75" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B76" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C76" t="n">
         <v>12</v>
       </c>
       <c r="D76" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E76" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B77" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C77" t="n">
         <v>12</v>
       </c>
       <c r="D77" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E77" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C78" t="n">
         <v>12</v>
       </c>
       <c r="D78" t="n">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="E78" t="n">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C79" t="n">
         <v>12</v>
       </c>
       <c r="D79" t="n">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="E79" t="n">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B80" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C80" t="n">
         <v>12</v>
       </c>
       <c r="D80" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E80" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B81" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C81" t="n">
         <v>12</v>
       </c>
       <c r="D81" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E81" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B82" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C82" t="n">
         <v>12</v>
       </c>
       <c r="D82" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E82" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B83" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C83" t="n">
         <v>12</v>
       </c>
       <c r="D83" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E83" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B84" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C84" t="n">
         <v>12</v>
       </c>
       <c r="D84" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="E84" t="n">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B85" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C85" t="n">
         <v>12</v>
       </c>
       <c r="D85" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E85" t="n">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B86" t="n">
         <v>8</v>
@@ -1899,15 +1899,15 @@
         <v>12</v>
       </c>
       <c r="D86" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E86" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B87" t="n">
         <v>8</v>
@@ -1916,10 +1916,10 @@
         <v>12</v>
       </c>
       <c r="D87" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E87" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -1927,13 +1927,13 @@
         <v>4</v>
       </c>
       <c r="B88" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C88" t="n">
         <v>12</v>
       </c>
       <c r="D88" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E88" t="n">
         <v>0.3</v>
@@ -1944,13 +1944,13 @@
         <v>4</v>
       </c>
       <c r="B89" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
         <v>12</v>
       </c>
       <c r="D89" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E89" t="n">
         <v>0.7</v>
@@ -1961,13 +1961,13 @@
         <v>4</v>
       </c>
       <c r="B90" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
         <v>12</v>
       </c>
       <c r="D90" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E90" t="n">
         <v>0.3</v>
@@ -1978,15 +1978,253 @@
         <v>4</v>
       </c>
       <c r="B91" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C91" t="n">
         <v>12</v>
       </c>
       <c r="D91" t="n">
+        <v>50</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>4</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>12</v>
+      </c>
+      <c r="D92" t="n">
         <v>200</v>
       </c>
-      <c r="E91" t="n">
+      <c r="E92" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>4</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+      <c r="C93" t="n">
+        <v>12</v>
+      </c>
+      <c r="D93" t="n">
+        <v>200</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>4</v>
+      </c>
+      <c r="B94" t="n">
+        <v>4</v>
+      </c>
+      <c r="C94" t="n">
+        <v>12</v>
+      </c>
+      <c r="D94" t="n">
+        <v>10</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>4</v>
+      </c>
+      <c r="B95" t="n">
+        <v>4</v>
+      </c>
+      <c r="C95" t="n">
+        <v>12</v>
+      </c>
+      <c r="D95" t="n">
+        <v>10</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>4</v>
+      </c>
+      <c r="B96" t="n">
+        <v>4</v>
+      </c>
+      <c r="C96" t="n">
+        <v>12</v>
+      </c>
+      <c r="D96" t="n">
+        <v>50</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>4</v>
+      </c>
+      <c r="B97" t="n">
+        <v>4</v>
+      </c>
+      <c r="C97" t="n">
+        <v>12</v>
+      </c>
+      <c r="D97" t="n">
+        <v>50</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>4</v>
+      </c>
+      <c r="B98" t="n">
+        <v>4</v>
+      </c>
+      <c r="C98" t="n">
+        <v>12</v>
+      </c>
+      <c r="D98" t="n">
+        <v>200</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>4</v>
+      </c>
+      <c r="B99" t="n">
+        <v>4</v>
+      </c>
+      <c r="C99" t="n">
+        <v>12</v>
+      </c>
+      <c r="D99" t="n">
+        <v>200</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>4</v>
+      </c>
+      <c r="B100" t="n">
+        <v>8</v>
+      </c>
+      <c r="C100" t="n">
+        <v>12</v>
+      </c>
+      <c r="D100" t="n">
+        <v>10</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>4</v>
+      </c>
+      <c r="B101" t="n">
+        <v>8</v>
+      </c>
+      <c r="C101" t="n">
+        <v>12</v>
+      </c>
+      <c r="D101" t="n">
+        <v>10</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>4</v>
+      </c>
+      <c r="B102" t="n">
+        <v>8</v>
+      </c>
+      <c r="C102" t="n">
+        <v>12</v>
+      </c>
+      <c r="D102" t="n">
+        <v>50</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>4</v>
+      </c>
+      <c r="B103" t="n">
+        <v>8</v>
+      </c>
+      <c r="C103" t="n">
+        <v>12</v>
+      </c>
+      <c r="D103" t="n">
+        <v>50</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>4</v>
+      </c>
+      <c r="B104" t="n">
+        <v>8</v>
+      </c>
+      <c r="C104" t="n">
+        <v>12</v>
+      </c>
+      <c r="D104" t="n">
+        <v>200</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>4</v>
+      </c>
+      <c r="B105" t="n">
+        <v>8</v>
+      </c>
+      <c r="C105" t="n">
+        <v>12</v>
+      </c>
+      <c r="D105" t="n">
+        <v>200</v>
+      </c>
+      <c r="E105" t="n">
         <v>0.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final test matrix version: louis
</commit_message>
<xml_diff>
--- a/Stability/wind_tunnel_test/wind_tunnel_test_matrix.xlsx
+++ b/Stability/wind_tunnel_test/wind_tunnel_test_matrix.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>